<commit_message>
Change self data item template handling
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/TotalsPanelRenderTest/TestPanelRenderWithParentContext.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/TotalsPanelRenderTest/TestPanelRenderWithParentContext.xlsx
@@ -91,7 +91,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -388,13 +388,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -402,7 +404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -410,7 +412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -418,26 +420,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>55.76</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -445,7 +450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -453,14 +458,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9">
+        <v>5500.8</v>
+      </c>
+      <c r="E9" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>